<commit_message>
updated exportToExcel() , output filename added more details. Will merge with main
</commit_message>
<xml_diff>
--- a/agenda_input.xlsx
+++ b/agenda_input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28110"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0025DE28-4BEA-4911-A182-B156274E1B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0433CF3E-4BDD-480E-9BCE-740A3A25B39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>Agenda Title:</t>
   </si>
   <si>
-    <t>Agenda Test</t>
+    <t>New agenda input</t>
   </si>
   <si>
     <t>Agenda Start-time</t>
@@ -364,7 +364,7 @@
   <dimension ref="A1:H1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -404,7 +404,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -432,7 +432,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -488,7 +488,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>

</xml_diff>